<commit_message>
ClinicAdmin-Patient-validate my treatments,Appointments-validate appointment details
</commit_message>
<xml_diff>
--- a/bin/test/ClinicAdmin_TestData/Watts Health Center/Patient-details.xlsx
+++ b/bin/test/ClinicAdmin_TestData/Watts Health Center/Patient-details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalDetails" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
   <si>
     <t>Patient_ID</t>
   </si>
@@ -144,6 +144,142 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>AppointmentDate</t>
+  </si>
+  <si>
+    <t>Oct 7, 2020</t>
+  </si>
+  <si>
+    <t>Oct 18, 2020 01:30 PM</t>
+  </si>
+  <si>
+    <t>Clinic Visit</t>
+  </si>
+  <si>
+    <t>General appointment</t>
+  </si>
+  <si>
+    <t>Oct 18, 2020</t>
+  </si>
+  <si>
+    <t>Oct 9, 2020</t>
+  </si>
+  <si>
+    <t>Oct 9, 2020 06:30 PM</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Oct 17, 2020</t>
+  </si>
+  <si>
+    <t>Oct 17, 2020 11:00 AM</t>
+  </si>
+  <si>
+    <t>Followup-General appointment</t>
+  </si>
+  <si>
+    <t>Followup comment and fee-1000</t>
+  </si>
+  <si>
+    <t>JPG-5MB.jpg</t>
+  </si>
+  <si>
+    <t>Oct 10, 2020</t>
+  </si>
+  <si>
+    <t>Report_name</t>
+  </si>
+  <si>
+    <t>Report_description</t>
+  </si>
+  <si>
+    <t>JPG-1MB.jpg,                                       JPG-5MB.jpg, 
+New Microsoft Excel Worksheet.xlsx</t>
+  </si>
+  <si>
+    <t>Oct 10, 2020 10:00 AM</t>
+  </si>
+  <si>
+    <t>No Documents uploaded</t>
+  </si>
+  <si>
+    <t>test,                                                  12,                                                    excel</t>
+  </si>
+  <si>
+    <t>Clinical Note</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
+  </si>
+  <si>
+    <t>ClinicalNote:Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
+  </si>
+  <si>
+    <t>Observation :Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
+  </si>
+  <si>
+    <t>Diagnosis :Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
+  </si>
+  <si>
+    <t>Drug Name</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Before/After</t>
+  </si>
+  <si>
+    <t>Dosage</t>
+  </si>
+  <si>
+    <t>After Food</t>
+  </si>
+  <si>
+    <t>Drug001/Drug002</t>
+  </si>
+  <si>
+    <t>100 ml/10 mg</t>
+  </si>
+  <si>
+    <t>1-1-1/ 1-0-0</t>
+  </si>
+  <si>
+    <t>5 Days/10 Days</t>
+  </si>
+  <si>
+    <t>After Food/ Before Food</t>
+  </si>
+  <si>
+    <t>Drug-005</t>
+  </si>
+  <si>
+    <t>10 mg</t>
+  </si>
+  <si>
+    <t>0-0-1</t>
+  </si>
+  <si>
+    <t>20 Days</t>
+  </si>
+  <si>
+    <t>No Clinical Note</t>
+  </si>
+  <si>
+    <t>No Observation</t>
+  </si>
+  <si>
+    <t>No Diagnosis</t>
   </si>
 </sst>
 </file>
@@ -181,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -204,11 +340,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -217,6 +364,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,7 +682,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,135 +878,658 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="2"/>
+      <c r="M2" s="2">
         <v>2000</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2">
+        <v>2000</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2">
+        <v>2000</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2">
+        <v>38</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2">
+        <v>70</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2">
+        <v>70</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2">
+        <v>70</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" customWidth="1"/>
+    <col min="6" max="6" width="57.28515625" customWidth="1"/>
+    <col min="7" max="7" width="46.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clinic Admin-Validation on appointment and invoice module
Clinic Admin-Validation on appointment and invoice module
</commit_message>
<xml_diff>
--- a/bin/test/ClinicAdmin_TestData/Watts Health Center/Patient-details.xlsx
+++ b/bin/test/ClinicAdmin_TestData/Watts Health Center/Patient-details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalDetails" sheetId="1" r:id="rId1"/>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1114,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>